<commit_message>
Fix stars calculation bug
</commit_message>
<xml_diff>
--- a/toilet data/stars.xlsx
+++ b/toilet data/stars.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\TF\tf\toilet data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AAF8CB-36A1-4955-BFD7-13AE381E9D9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D11A18-BD69-41D2-9127-EBBE449FCF5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9058807A-4CBC-40CD-8BB5-A8811CB9D5EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{9058807A-4CBC-40CD-8BB5-A8811CB9D5EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,12 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>star</t>
   </si>
   <si>
     <t>num</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -388,2235 +390,3069 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0563866D-553B-433E-B44C-BD79F58D4048}">
-  <dimension ref="A1:B278"/>
+  <dimension ref="A1:C278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A278"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C278"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1</v>
       </c>
       <c r="B50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1</v>
       </c>
       <c r="B53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1</v>
       </c>
       <c r="B64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1</v>
       </c>
       <c r="B66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1</v>
       </c>
       <c r="B68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
       <c r="B69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1</v>
       </c>
       <c r="B70">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
       <c r="B71">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
       <c r="B72">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1</v>
       </c>
       <c r="B74">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
       <c r="B75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1</v>
       </c>
       <c r="B77">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1</v>
       </c>
       <c r="B78">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1</v>
       </c>
       <c r="B80">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1</v>
       </c>
       <c r="B82">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1</v>
       </c>
       <c r="B83">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1</v>
       </c>
       <c r="B84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1</v>
       </c>
       <c r="B86">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1</v>
       </c>
       <c r="B87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1</v>
       </c>
       <c r="B88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1</v>
       </c>
       <c r="B89">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1</v>
       </c>
       <c r="B90">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1</v>
       </c>
       <c r="B91">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1</v>
       </c>
       <c r="B92">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1</v>
       </c>
       <c r="B93">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1</v>
       </c>
       <c r="B94">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1</v>
       </c>
       <c r="B96">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1</v>
       </c>
       <c r="B97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1</v>
       </c>
       <c r="B98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>1</v>
       </c>
       <c r="B99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1</v>
       </c>
       <c r="B100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1</v>
       </c>
       <c r="B101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1</v>
       </c>
       <c r="B102">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1</v>
       </c>
       <c r="B103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1</v>
       </c>
       <c r="B104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1</v>
       </c>
       <c r="B106">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1</v>
       </c>
       <c r="B107">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>1</v>
       </c>
       <c r="B108">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1</v>
       </c>
       <c r="B109">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1</v>
       </c>
       <c r="B110">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1</v>
       </c>
       <c r="B111">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1</v>
       </c>
       <c r="B113">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>1</v>
       </c>
       <c r="B114">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1</v>
       </c>
       <c r="B115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1</v>
       </c>
       <c r="B117">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1</v>
       </c>
       <c r="B118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1</v>
       </c>
       <c r="B119">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1</v>
       </c>
       <c r="B120">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1</v>
       </c>
       <c r="B121">
         <v>3</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>1</v>
       </c>
       <c r="B122">
         <v>3</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>1</v>
       </c>
       <c r="B123">
         <v>3</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>1</v>
       </c>
       <c r="B124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1</v>
       </c>
       <c r="B125">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>1</v>
       </c>
       <c r="B126">
         <v>3</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>1</v>
       </c>
       <c r="B127">
         <v>3</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>1</v>
       </c>
       <c r="B128">
         <v>3</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>1</v>
       </c>
       <c r="B129">
         <v>3</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>1</v>
       </c>
       <c r="B130">
         <v>3</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>1</v>
       </c>
       <c r="B131">
         <v>3</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>1</v>
       </c>
       <c r="B132">
         <v>3</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>1</v>
       </c>
       <c r="B133">
         <v>3</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>1</v>
       </c>
       <c r="B134">
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>1</v>
       </c>
       <c r="B135">
         <v>3</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>1</v>
       </c>
       <c r="B136">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>1</v>
       </c>
       <c r="B137">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>1</v>
       </c>
       <c r="B138">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>1</v>
       </c>
       <c r="B139">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>1</v>
       </c>
       <c r="B140">
         <v>3</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>1</v>
       </c>
       <c r="B141">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>1</v>
       </c>
       <c r="B142">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>1</v>
       </c>
       <c r="B143">
         <v>3</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>1</v>
       </c>
       <c r="B144">
         <v>3</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>1</v>
       </c>
       <c r="B145">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>1</v>
       </c>
       <c r="B146">
         <v>3</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>1</v>
       </c>
       <c r="B147">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>1</v>
       </c>
       <c r="B148">
         <v>3</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>1</v>
       </c>
       <c r="B149">
         <v>3</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>1</v>
       </c>
       <c r="B150">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>1</v>
       </c>
       <c r="B151">
         <v>3</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>1</v>
       </c>
       <c r="B152">
         <v>3</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>1</v>
       </c>
       <c r="B153">
         <v>3</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>1</v>
       </c>
       <c r="B154">
         <v>3</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>1</v>
       </c>
       <c r="B155">
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>1</v>
       </c>
       <c r="B156">
         <v>3</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>1</v>
       </c>
       <c r="B157">
         <v>3</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>1</v>
       </c>
       <c r="B158">
         <v>3</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>1</v>
       </c>
       <c r="B159">
         <v>3</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>1</v>
       </c>
       <c r="B160">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>1</v>
       </c>
       <c r="B161">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>1</v>
       </c>
       <c r="B162">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>1</v>
       </c>
       <c r="B163">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>1</v>
       </c>
       <c r="B164">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>1</v>
       </c>
       <c r="B165">
         <v>3</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>1</v>
       </c>
       <c r="B166">
         <v>3</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>1</v>
       </c>
       <c r="B167">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>1</v>
       </c>
       <c r="B168">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>1</v>
       </c>
       <c r="B169">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>1</v>
       </c>
       <c r="B170">
         <v>3</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>1</v>
       </c>
       <c r="B171">
         <v>3</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>1</v>
       </c>
       <c r="B172">
         <v>3</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>1</v>
       </c>
       <c r="B173">
         <v>3</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>1</v>
       </c>
       <c r="B174">
         <v>3</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>1</v>
       </c>
       <c r="B175">
         <v>3</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>1</v>
       </c>
       <c r="B176">
         <v>3</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>1</v>
       </c>
       <c r="B177">
         <v>3</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>1</v>
       </c>
       <c r="B178">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>1</v>
       </c>
       <c r="B179">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>1</v>
       </c>
       <c r="B180">
         <v>3</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>1</v>
       </c>
       <c r="B181">
         <v>3</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>1</v>
       </c>
       <c r="B182">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>1</v>
       </c>
       <c r="B183">
         <v>3</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>1</v>
       </c>
       <c r="B184">
         <v>3</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>1</v>
       </c>
       <c r="B185">
         <v>3</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>1</v>
       </c>
       <c r="B186">
         <v>3</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>1</v>
       </c>
       <c r="B187">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>1</v>
       </c>
       <c r="B188">
         <v>3</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>1</v>
       </c>
       <c r="B189">
         <v>3</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>1</v>
       </c>
       <c r="B190">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>1</v>
       </c>
       <c r="B191">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>1</v>
       </c>
       <c r="B192">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>1</v>
       </c>
       <c r="B193">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>1</v>
       </c>
       <c r="B194">
         <v>3</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>1</v>
       </c>
       <c r="B195">
         <v>3</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>1</v>
       </c>
       <c r="B196">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>1</v>
       </c>
       <c r="B197">
         <v>3</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>1</v>
       </c>
       <c r="B198">
         <v>3</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>1</v>
       </c>
       <c r="B199">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>1</v>
       </c>
       <c r="B200">
         <v>3</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>1</v>
       </c>
       <c r="B201">
         <v>3</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>1</v>
       </c>
       <c r="B202">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>1</v>
       </c>
       <c r="B203">
         <v>3</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>1</v>
       </c>
       <c r="B204">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>1</v>
       </c>
       <c r="B205">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>1</v>
       </c>
       <c r="B206">
         <v>3</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>1</v>
       </c>
       <c r="B207">
         <v>3</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>1</v>
       </c>
       <c r="B208">
         <v>3</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>1</v>
       </c>
       <c r="B209">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>1</v>
       </c>
       <c r="B210">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>1</v>
       </c>
       <c r="B211">
         <v>3</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>1</v>
       </c>
       <c r="B212">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>1</v>
       </c>
       <c r="B213">
         <v>3</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>1</v>
       </c>
       <c r="B214">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>1</v>
       </c>
       <c r="B215">
         <v>3</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>1</v>
       </c>
       <c r="B216">
         <v>3</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>1</v>
       </c>
       <c r="B217">
         <v>3</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>1</v>
       </c>
       <c r="B218">
         <v>3</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>1</v>
       </c>
       <c r="B219">
         <v>3</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>1</v>
       </c>
       <c r="B220">
         <v>3</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>1</v>
       </c>
       <c r="B221">
         <v>3</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>1</v>
       </c>
       <c r="B222">
         <v>3</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>1</v>
       </c>
       <c r="B223">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>1</v>
       </c>
       <c r="B224">
         <v>3</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>1</v>
       </c>
       <c r="B225">
         <v>3</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>1</v>
       </c>
       <c r="B226">
         <v>3</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>1</v>
       </c>
       <c r="B227">
         <v>3</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>1</v>
       </c>
       <c r="B228">
         <v>3</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>1</v>
       </c>
       <c r="B229">
         <v>3</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>1</v>
       </c>
       <c r="B230">
         <v>3</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>1</v>
       </c>
       <c r="B231">
         <v>3</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>1</v>
       </c>
       <c r="B232">
         <v>3</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>1</v>
       </c>
       <c r="B233">
         <v>3</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>1</v>
       </c>
       <c r="B234">
         <v>3</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>1</v>
       </c>
       <c r="B235">
         <v>3</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>1</v>
       </c>
       <c r="B236">
         <v>3</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>1</v>
       </c>
       <c r="B237">
         <v>3</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>1</v>
       </c>
       <c r="B238">
         <v>3</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>1</v>
       </c>
       <c r="B239">
         <v>3</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>1</v>
       </c>
       <c r="B240">
         <v>3</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>1</v>
       </c>
       <c r="B241">
         <v>3</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>1</v>
       </c>
       <c r="B242">
         <v>3</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>1</v>
       </c>
       <c r="B243">
         <v>3</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C243">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>1</v>
       </c>
       <c r="B244">
         <v>3</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>1</v>
       </c>
       <c r="B245">
         <v>3</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>1</v>
       </c>
       <c r="B246">
         <v>3</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>1</v>
       </c>
       <c r="B247">
         <v>3</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>1</v>
       </c>
       <c r="B248">
         <v>3</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>1</v>
       </c>
       <c r="B249">
         <v>3</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>1</v>
       </c>
       <c r="B250">
         <v>3</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C250">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>1</v>
       </c>
       <c r="B251">
         <v>3</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>1</v>
       </c>
       <c r="B252">
         <v>3</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>1</v>
       </c>
       <c r="B253">
         <v>3</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>1</v>
       </c>
       <c r="B254">
         <v>3</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>1</v>
       </c>
       <c r="B255">
         <v>3</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C255">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>1</v>
       </c>
       <c r="B256">
         <v>3</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>1</v>
       </c>
       <c r="B257">
         <v>3</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C257">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>1</v>
       </c>
       <c r="B258">
         <v>3</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C258">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>1</v>
       </c>
       <c r="B259">
         <v>3</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C259">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>1</v>
       </c>
       <c r="B260">
         <v>3</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C260">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>1</v>
       </c>
       <c r="B261">
         <v>3</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>1</v>
       </c>
       <c r="B262">
         <v>3</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>1</v>
       </c>
       <c r="B263">
         <v>3</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>1</v>
       </c>
       <c r="B264">
         <v>3</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>1</v>
       </c>
       <c r="B265">
         <v>3</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>1</v>
       </c>
       <c r="B266">
         <v>3</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C266">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>1</v>
       </c>
       <c r="B267">
         <v>3</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>1</v>
       </c>
       <c r="B268">
         <v>3</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>1</v>
       </c>
       <c r="B269">
         <v>3</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>1</v>
       </c>
       <c r="B270">
         <v>3</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>1</v>
       </c>
       <c r="B271">
         <v>3</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>1</v>
       </c>
       <c r="B272">
         <v>3</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>1</v>
       </c>
       <c r="B273">
         <v>3</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>1</v>
       </c>
       <c r="B274">
         <v>3</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>1</v>
       </c>
       <c r="B275">
         <v>3</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>1</v>
       </c>
       <c r="B276">
         <v>3</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>1</v>
       </c>
       <c r="B277">
         <v>3</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>1</v>
       </c>
       <c r="B278">
+        <v>3</v>
+      </c>
+      <c r="C278">
         <v>3</v>
       </c>
     </row>

</xml_diff>